<commit_message>
adds final xlsx files
</commit_message>
<xml_diff>
--- a/Assignment_3/accuracies-over-epochs-5.xlsx
+++ b/Assignment_3/accuracies-over-epochs-5.xlsx
@@ -1485,11 +1485,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-576975904"/>
-        <c:axId val="-645029456"/>
+        <c:axId val="1845156080"/>
+        <c:axId val="1845158400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-576975904"/>
+        <c:axId val="1845156080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1532,7 +1532,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-645029456"/>
+        <c:crossAx val="1845158400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1540,7 +1540,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-645029456"/>
+        <c:axId val="1845158400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.83"/>
@@ -1592,7 +1592,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-576975904"/>
+        <c:crossAx val="1845156080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2244,15 +2244,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>107950</xdr:colOff>
+      <xdr:colOff>101600</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>